<commit_message>
IFS Upgrade - Recent
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lavanya.rajaram\Documents\IFS UPGRADE RPA\VPN 14\IFS_Upgrade_Project-master\IFS_Upgrade_Project-master\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\IFS_Upgrade_Project-master\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7C2234-D0E7-43EB-B1E7-29F0708B151D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E0351B-9B7E-4C60-8143-A8251419AE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,9 +214,6 @@
     <t>Downloads</t>
   </si>
   <si>
-    <t>192.168.2.15</t>
-  </si>
-  <si>
     <t>D:\IFS\Logs\Prepare DB</t>
   </si>
   <si>
@@ -227,6 +224,9 @@
   </si>
   <si>
     <t>\\DT-PROV-ASUS18\Doc_Temp_Path</t>
+  </si>
+  <si>
+    <t>192.168.2.14</t>
   </si>
 </sst>
 </file>
@@ -610,9 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -661,7 +659,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -741,7 +739,7 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -757,7 +755,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -797,7 +795,7 @@
         <v>43</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -877,7 +875,7 @@
         <v>53</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>